<commit_message>
New setup added of screenshot, testCaseFolderCreation
</commit_message>
<xml_diff>
--- a/src/test/resources/data/TestingAutomationExcelSheet.xlsx
+++ b/src/test/resources/data/TestingAutomationExcelSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Automation_Testing\health-care-test-automation\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C01A887-F7D9-47A8-8ED6-2BE45A999C5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BC812E4-6086-45E4-8F88-48A4F5A6B8D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A81CDDE0-A704-4C59-B347-98BC9129A736}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="24">
   <si>
     <t>Executer</t>
   </si>
@@ -107,6 +107,9 @@
   </si>
   <si>
     <t>test1@gmail.com</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -512,7 +515,7 @@
   <dimension ref="A2:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15:K16"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -559,7 +562,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>21</v>
@@ -584,7 +587,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
implement profile page and update profile functionality
</commit_message>
<xml_diff>
--- a/src/test/resources/data/TestingAutomationExcelSheet.xlsx
+++ b/src/test/resources/data/TestingAutomationExcelSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Automation_Testing\health-care-test-automation\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E178E1E6-1E2B-485F-AEE0-808CC6287C72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18AA8954-ED54-4F8B-AE7F-B9BF990E510B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A81CDDE0-A704-4C59-B347-98BC9129A736}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$B$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$C$4:$C$5</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="51">
   <si>
     <t>Executer</t>
   </si>
@@ -137,6 +137,60 @@
   </si>
   <si>
     <t>My Appointments</t>
+  </si>
+  <si>
+    <t>My Profile</t>
+  </si>
+  <si>
+    <t>Updated Name</t>
+  </si>
+  <si>
+    <t>Updated Address Lane 1</t>
+  </si>
+  <si>
+    <t>Updated Address Lane 2</t>
+  </si>
+  <si>
+    <t>Updated Image URL</t>
+  </si>
+  <si>
+    <t>Updated Gender</t>
+  </si>
+  <si>
+    <t>Updated DOB</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>My Appointments Page Testing</t>
+  </si>
+  <si>
+    <t>Book Appointment Testing</t>
+  </si>
+  <si>
+    <t>My Profile Page Testing</t>
+  </si>
+  <si>
+    <t>DSF HJD</t>
+  </si>
+  <si>
+    <t>C Wing 3rd Floor</t>
+  </si>
+  <si>
+    <t>XYZ Apartment, Paris</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Update Profile</t>
+  </si>
+  <si>
+    <t>"E:\Backgrounds\bg-2.jpg"</t>
+  </si>
+  <si>
+    <t>17-08-2001</t>
   </si>
 </sst>
 </file>
@@ -168,7 +222,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -178,6 +232,66 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -210,7 +324,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -218,16 +332,52 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -545,183 +695,310 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE8C265A-30CE-4F6B-A0B8-C55CE50459EC}">
-  <dimension ref="A2:O4"/>
+  <dimension ref="A2:X16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="8.88671875" style="8"/>
-    <col min="3" max="3" width="9.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.109375" style="8" customWidth="1"/>
-    <col min="5" max="5" width="8.88671875" style="8"/>
-    <col min="6" max="6" width="24.77734375" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.77734375" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.77734375" style="8" customWidth="1"/>
-    <col min="10" max="10" width="15.5546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.5546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.77734375" style="8" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.77734375" style="8" customWidth="1"/>
-    <col min="15" max="15" width="16.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="8.88671875" style="8"/>
+    <col min="1" max="1" width="8.77734375" style="5" customWidth="1"/>
+    <col min="2" max="2" width="26.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="5"/>
+    <col min="4" max="4" width="9.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.109375" style="5" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="5"/>
+    <col min="7" max="7" width="24.77734375" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.77734375" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.77734375" style="5" customWidth="1"/>
+    <col min="11" max="11" width="15.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.77734375" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.77734375" style="5" customWidth="1"/>
+    <col min="16" max="17" width="16.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.33203125" style="5" customWidth="1"/>
+    <col min="19" max="19" width="16.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="21.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="22.77734375" style="5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="18" style="5" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="25.77734375" style="20" bestFit="1" customWidth="1"/>
+    <col min="25" max="16384" width="8.88671875" style="5"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="J2" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="K2" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="L2" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="M2" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="N2" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="O2" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="P2" s="14" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" s="5">
+      <c r="Q2" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="R2" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="S2" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="T2" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="U2" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="V2" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="W2" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="X2" s="18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A3" s="16">
         <v>1</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" s="6">
+        <v>700</v>
+      </c>
+      <c r="M3" s="6">
+        <v>28</v>
+      </c>
+      <c r="N3" s="7">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="O3" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="P3" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="Q3" s="9"/>
+      <c r="R3" s="9"/>
+      <c r="S3" s="9"/>
+      <c r="T3" s="9"/>
+      <c r="U3" s="9"/>
+      <c r="V3" s="9"/>
+      <c r="W3" s="9"/>
+      <c r="X3" s="19"/>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A4" s="16">
+        <v>2</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="E4" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="F4" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="K3" s="5">
-        <v>700</v>
-      </c>
-      <c r="L3" s="5">
-        <v>28</v>
-      </c>
-      <c r="M3" s="7">
-        <v>0.52083333333333337</v>
-      </c>
-      <c r="N3" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="O3" s="5" t="s">
+      <c r="G4" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="J4" s="6" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" s="5">
-        <v>2</v>
-      </c>
-      <c r="B4" s="5" t="s">
+      <c r="K4" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="L4" s="6">
+        <v>649</v>
+      </c>
+      <c r="M4" s="6">
+        <v>15</v>
+      </c>
+      <c r="N4" s="7">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="O4" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="P4" s="8"/>
+      <c r="Q4" s="9"/>
+      <c r="R4" s="9"/>
+      <c r="S4" s="9"/>
+      <c r="T4" s="9"/>
+      <c r="U4" s="9"/>
+      <c r="V4" s="9"/>
+      <c r="W4" s="9"/>
+      <c r="X4" s="19"/>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A5" s="16">
+        <v>3</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="L5" s="6">
+        <v>649</v>
+      </c>
+      <c r="M5" s="6">
+        <v>5</v>
+      </c>
+      <c r="N5" s="7">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="O5" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="P5" s="8"/>
+      <c r="Q5" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="I4" s="5" t="s">
+      <c r="R5" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="J4" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="K4" s="5">
-        <v>649</v>
-      </c>
-      <c r="L4" s="5">
-        <v>5</v>
-      </c>
-      <c r="M4" s="7">
-        <v>0.45833333333333331</v>
-      </c>
-      <c r="N4" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="O4" s="5" t="s">
-        <v>2</v>
-      </c>
+      <c r="S5" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="T5" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="U5" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="V5" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="W5" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="X5" s="19" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="J16" s="10"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:B18" xr:uid="{CE8C265A-30CE-4F6B-A0B8-C55CE50459EC}"/>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1" xr:uid="{4956BE33-23E8-4A30-9BE2-A8884E71D382}"/>
-    <hyperlink ref="D4" r:id="rId2" display="atishay@gmail.com" xr:uid="{7344DD6E-2CD2-49FB-83A8-4BE294AEF7E9}"/>
-    <hyperlink ref="D4" r:id="rId3" xr:uid="{D356A526-19D1-4756-95A4-D43C85951E59}"/>
-    <hyperlink ref="F3" r:id="rId4" xr:uid="{5A80F9A3-DF0D-4097-A0AD-BE1FB1AFCB02}"/>
-    <hyperlink ref="F4" r:id="rId5" xr:uid="{1DBF47D1-9D4D-4233-B25A-FA3750536FC4}"/>
+    <hyperlink ref="E3" r:id="rId1" xr:uid="{4956BE33-23E8-4A30-9BE2-A8884E71D382}"/>
+    <hyperlink ref="E4" r:id="rId2" display="atishay@gmail.com" xr:uid="{7344DD6E-2CD2-49FB-83A8-4BE294AEF7E9}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{D356A526-19D1-4756-95A4-D43C85951E59}"/>
+    <hyperlink ref="G3" r:id="rId4" xr:uid="{5A80F9A3-DF0D-4097-A0AD-BE1FB1AFCB02}"/>
+    <hyperlink ref="G4" r:id="rId5" xr:uid="{1DBF47D1-9D4D-4233-B25A-FA3750536FC4}"/>
+    <hyperlink ref="E5" r:id="rId6" xr:uid="{4C200619-807B-45C0-909A-D6F4DFF578B9}"/>
+    <hyperlink ref="G5" r:id="rId7" xr:uid="{62E397E4-8A6E-4034-B35C-2826E3F61F71}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
implement my appointments page and added upload files functionality
</commit_message>
<xml_diff>
--- a/src/test/resources/data/TestingAutomationExcelSheet.xlsx
+++ b/src/test/resources/data/TestingAutomationExcelSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Automation_Testing\health-care-test-automation\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18AA8954-ED54-4F8B-AE7F-B9BF990E510B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BDE7C9B-FBBF-49A8-83E0-BFD9AAA9C55B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A81CDDE0-A704-4C59-B347-98BC9129A736}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$C$4:$C$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$C$2:$C$5</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="53">
   <si>
     <t>Executer</t>
   </si>
@@ -151,9 +151,6 @@
     <t>Updated Address Lane 2</t>
   </si>
   <si>
-    <t>Updated Image URL</t>
-  </si>
-  <si>
     <t>Updated Gender</t>
   </si>
   <si>
@@ -187,10 +184,19 @@
     <t>Update Profile</t>
   </si>
   <si>
-    <t>"E:\Backgrounds\bg-2.jpg"</t>
-  </si>
-  <si>
     <t>17-08-2001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Update Image</t>
+  </si>
+  <si>
+    <t>profile-pic.png</t>
+  </si>
+  <si>
+    <t>ImageFile Name</t>
   </si>
 </sst>
 </file>
@@ -695,10 +701,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE8C265A-30CE-4F6B-A0B8-C55CE50459EC}">
-  <dimension ref="A2:X16"/>
+  <dimension ref="A1:Y16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -722,18 +728,24 @@
     <col min="18" max="18" width="16.33203125" style="5" customWidth="1"/>
     <col min="19" max="19" width="16.33203125" style="5" bestFit="1" customWidth="1"/>
     <col min="20" max="21" width="21.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="22.77734375" style="5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="18" style="5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="25.77734375" style="20" bestFit="1" customWidth="1"/>
-    <col min="25" max="16384" width="8.88671875" style="5"/>
+    <col min="22" max="22" width="21.6640625" style="5" customWidth="1"/>
+    <col min="23" max="23" width="22.77734375" style="5" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18" style="5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="25.77734375" style="20" bestFit="1" customWidth="1"/>
+    <col min="26" max="16384" width="8.88671875" style="5"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="T1" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>0</v>
@@ -781,7 +793,7 @@
         <v>33</v>
       </c>
       <c r="R2" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="S2" s="11" t="s">
         <v>34</v>
@@ -793,24 +805,27 @@
         <v>36</v>
       </c>
       <c r="V2" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="W2" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="X2" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="W2" s="11" t="s">
+      <c r="Y2" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="X2" s="18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" s="16">
         <v>1</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="D3" s="16" t="s">
         <v>21</v>
@@ -856,14 +871,15 @@
       <c r="U3" s="9"/>
       <c r="V3" s="9"/>
       <c r="W3" s="9"/>
-      <c r="X3" s="19"/>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X3" s="9"/>
+      <c r="Y3" s="19"/>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A4" s="16">
         <v>2</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C4" s="16" t="s">
         <v>2</v>
@@ -912,14 +928,15 @@
       <c r="U4" s="9"/>
       <c r="V4" s="9"/>
       <c r="W4" s="9"/>
-      <c r="X4" s="19"/>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X4" s="9"/>
+      <c r="Y4" s="19"/>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A5" s="16">
         <v>3</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C5" s="16" t="s">
         <v>2</v>
@@ -966,25 +983,28 @@
         <v>22</v>
       </c>
       <c r="S5" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="T5" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="T5" s="9" t="s">
+      <c r="U5" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="U5" s="9" t="s">
+      <c r="V5" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="W5" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="X5" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="V5" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="W5" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="X5" s="19" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y5" s="19" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
       <c r="J16" s="10"/>
     </row>
   </sheetData>

</xml_diff>